<commit_message>
Breakpoint may never be perfect
</commit_message>
<xml_diff>
--- a/usage.xlsx
+++ b/usage.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Website\CTEC3905-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{4AAB831C-AC7F-436B-A407-5AB40766A472}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$A$10</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>Usage</t>
   </si>
@@ -70,11 +74,14 @@
   <si>
     <t>Higher</t>
   </si>
+  <si>
+    <t>H</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,7 +100,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,6 +110,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -119,11 +132,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,6 +360,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-9F74-4C3F-B34E-8BC019488497}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -385,6 +404,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-9F74-4C3F-B34E-8BC019488497}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -402,6 +426,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-9F74-4C3F-B34E-8BC019488497}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -419,6 +448,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-9F74-4C3F-B34E-8BC019488497}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -436,6 +470,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-9F74-4C3F-B34E-8BC019488497}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -594,6 +633,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -601,7 +641,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -713,6 +752,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-70AF-4A74-A3E4-47B07AB7000D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -728,6 +772,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-70AF-4A74-A3E4-47B07AB7000D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -743,6 +792,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-70AF-4A74-A3E4-47B07AB7000D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -758,6 +812,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-70AF-4A74-A3E4-47B07AB7000D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -773,6 +832,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-70AF-4A74-A3E4-47B07AB7000D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -788,6 +852,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-70AF-4A74-A3E4-47B07AB7000D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -805,6 +874,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-70AF-4A74-A3E4-47B07AB7000D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -923,6 +997,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -930,7 +1005,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2456,11 +2530,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE929BD-BBAB-4EF5-8F35-830874C59555}">
-  <dimension ref="A1:B26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2468,7 +2542,7 @@
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2476,87 +2550,105 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="3">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -2564,7 +2656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -2572,15 +2664,15 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
     </row>
@@ -2661,4 +2753,69 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1200</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A10">
+    <sortState ref="A2:A10">
+      <sortCondition ref="A1:A10"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated README with new screen resolution information
</commit_message>
<xml_diff>
--- a/usage.xlsx
+++ b/usage.xlsx
@@ -13,11 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$A$10</definedName>
-  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Usage</t>
   </si>
@@ -64,9 +60,6 @@
   </si>
   <si>
     <t>1536x864</t>
-  </si>
-  <si>
-    <t>lower</t>
   </si>
   <si>
     <t>Higher</t>
@@ -113,7 +106,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,18 +115,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -141,19 +128,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -218,7 +221,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.825329613179618E-2"/>
+          <c:y val="0.1563919727425376"/>
+          <c:w val="0.48434557827193497"/>
+          <c:h val="0.85870489593056187"/>
+        </c:manualLayout>
+      </c:layout>
       <c:pieChart>
         <c:varyColors val="1"/>
         <c:ser>
@@ -226,7 +239,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -258,7 +271,6 @@
           <c:dPt>
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -279,7 +291,6 @@
           <c:dPt>
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
@@ -300,7 +311,6 @@
           <c:dPt>
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="4"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
@@ -321,7 +331,6 @@
           <c:dPt>
             <c:idx val="4"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
@@ -342,7 +351,6 @@
           <c:dPt>
             <c:idx val="5"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -363,7 +371,6 @@
           <c:dPt>
             <c:idx val="6"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1">
@@ -510,6 +517,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-1353-4F76-8B1A-B14C49C64A9E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -528,6 +540,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-1353-4F76-8B1A-B14C49C64A9E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -546,10 +563,15 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-1353-4F76-8B1A-B14C49C64A9E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$16</c:f>
+              <c:f>Sheet1!$B$3:$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -602,7 +624,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$16</c:f>
+              <c:f>Sheet1!$C$3:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="15"/>
@@ -685,10 +707,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.8952630425260753E-2"/>
-          <c:y val="0.88537903350316505"/>
-          <c:w val="0.90733251233117895"/>
-          <c:h val="0.11388878293327527"/>
+          <c:x val="0.62653780430728234"/>
+          <c:y val="0.17492215646957171"/>
+          <c:w val="0.29635400675724655"/>
+          <c:h val="0.70817457817772766"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -818,12 +840,9 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$20</c:f>
+              <c:f>Sheet1!$C$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Usage</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -970,61 +989,20 @@
             </c:extLst>
           </c:dPt>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$21:$A$27</c:f>
-              <c:strCache>
+            <c:numRef>
+              <c:f>Sheet1!$B$22:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Higher</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1920x1080</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1366x768</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1280x1024</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1280x800</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1024x768</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>lower</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$21:$B$27</c:f>
+              <c:f>Sheet1!$C$22:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>31.6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.4000000000000004</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2251,14 +2229,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>385762</xdr:colOff>
+      <xdr:colOff>61913</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>257175</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2286,15 +2264,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>409574</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>342899</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2620,291 +2598,386 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A14"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4">
-        <v>0.08</v>
-      </c>
+      <c r="C4" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4">
-        <v>0.06</v>
-      </c>
+      <c r="C10" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="6">
         <v>0.05</v>
       </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="6">
         <v>0.04</v>
       </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6">
         <v>0.03</v>
       </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0.02</v>
-      </c>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6">
+        <v>4.4000000000000004E-2</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0.02</v>
-      </c>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0.01</v>
-      </c>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0.01</v>
-      </c>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="5">
-        <v>0.17</v>
-      </c>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5">
-        <v>0.35</v>
-      </c>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="5">
-        <v>0.05</v>
-      </c>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C23" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="5">
-        <v>0.04</v>
-      </c>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="5">
-        <v>0.03</v>
-      </c>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="5">
-        <v>4.4000000000000004E-2</v>
-      </c>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="6"/>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="2">
-        <v>31.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="2">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="2">
-        <v>4.4000000000000004</v>
-      </c>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1200</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:A10">
-    <sortState ref="A2:A10">
-      <sortCondition ref="A1:A10"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Breakpoint tuning for final submission
</commit_message>
<xml_diff>
--- a/usage.xlsx
+++ b/usage.xlsx
@@ -148,7 +148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -157,6 +157,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2601,7 +2602,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2662,7 +2663,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="6">
@@ -2680,7 +2681,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="6">
@@ -2698,7 +2699,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="6">
@@ -2716,7 +2717,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="6">
@@ -2734,7 +2735,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="6">
@@ -2752,7 +2753,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="6">
@@ -2770,7 +2771,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="6">
@@ -2788,7 +2789,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="6">
@@ -2806,7 +2807,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="6">
@@ -2824,7 +2825,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="6">
@@ -2842,7 +2843,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="6">
@@ -2860,7 +2861,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="6">
@@ -2878,7 +2879,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="6">

</xml_diff>